<commit_message>
Update data in LOD calculator
</commit_message>
<xml_diff>
--- a/Scores/LOD.xlsx
+++ b/Scores/LOD.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomhsiung/Reference/Scores/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A00017B6-83C4-AF41-838D-2D2036F7E836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9512842C-02D2-3A4A-82B5-4904D1CFD30C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15320" yWindow="2640" windowWidth="11840" windowHeight="11900" xr2:uid="{662023FA-49DD-1F44-8785-01C9F7A40D2D}"/>
+    <workbookView xWindow="24580" yWindow="5960" windowWidth="11840" windowHeight="11900" xr2:uid="{662023FA-49DD-1F44-8785-01C9F7A40D2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -413,7 +413,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>